<commit_message>
Corrigido código de extração do estado
</commit_message>
<xml_diff>
--- a/Dados/Leiloeiros_MG.xlsx
+++ b/Dados/Leiloeiros_MG.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -500,7 +500,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -527,7 +527,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -554,7 +554,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -608,7 +608,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -793,7 +793,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -820,7 +820,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -874,7 +874,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -901,7 +901,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -928,7 +928,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -955,7 +955,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -982,7 +982,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1032,7 +1032,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1271,7 +1271,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>DF</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1425,7 +1425,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>DF</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1610,7 +1610,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1637,7 +1637,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1718,7 +1718,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1745,7 +1745,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1853,7 +1853,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1880,7 +1880,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1934,7 +1934,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2015,7 +2015,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2069,7 +2069,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2150,7 +2150,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2177,7 +2177,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2204,7 +2204,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>RN</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2339,7 +2339,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2393,7 +2393,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2420,7 +2420,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2474,7 +2474,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2528,7 +2528,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2555,7 +2555,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2609,7 +2609,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2636,7 +2636,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2663,7 +2663,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2690,7 +2690,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2717,7 +2717,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2740,7 +2740,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2767,7 +2767,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2848,7 +2848,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2875,7 +2875,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2902,7 +2902,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>PR</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2956,7 +2956,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2983,7 +2983,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -3010,7 +3010,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3064,7 +3064,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3118,7 +3118,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3145,7 +3145,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3172,7 +3172,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3199,7 +3199,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3226,7 +3226,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3253,7 +3253,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3280,7 +3280,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3307,7 +3307,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3334,7 +3334,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3415,7 +3415,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3442,7 +3442,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3469,7 +3469,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3496,7 +3496,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3523,7 +3523,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3550,7 +3550,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3658,7 +3658,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3685,7 +3685,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3712,7 +3712,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3739,7 +3739,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3766,7 +3766,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3793,7 +3793,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3901,7 +3901,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3928,7 +3928,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3955,7 +3955,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3982,7 +3982,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -4009,7 +4009,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -4036,7 +4036,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4090,7 +4090,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>DF</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4144,7 +4144,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4171,7 +4171,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4198,7 +4198,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4225,7 +4225,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4252,7 +4252,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4279,7 +4279,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4306,7 +4306,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4333,7 +4333,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4360,7 +4360,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4383,7 +4383,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4410,7 +4410,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4437,7 +4437,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4464,7 +4464,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -4491,7 +4491,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -4518,7 +4518,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -4545,7 +4545,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -4572,7 +4572,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -4599,7 +4599,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -4653,7 +4653,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -4680,7 +4680,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -4707,7 +4707,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -4734,7 +4734,7 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -4761,7 +4761,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -4784,7 +4784,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -4811,7 +4811,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -4865,7 +4865,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -4892,7 +4892,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -4946,7 +4946,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -4973,7 +4973,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -5000,7 +5000,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -5027,7 +5027,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -5054,7 +5054,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -5081,7 +5081,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -5108,7 +5108,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -5135,7 +5135,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -5162,7 +5162,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -5216,7 +5216,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -5243,7 +5243,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -5270,7 +5270,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -5297,7 +5297,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -5324,7 +5324,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -5351,7 +5351,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -5378,7 +5378,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">

</xml_diff>